<commit_message>
figures and gene expression analysis
</commit_message>
<xml_diff>
--- a/physiology/extra stats in case.xlsx
+++ b/physiology/extra stats in case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://miamiedu-my.sharepoint.com/personal/and128_miami_edu/Documents/GitHub/Ch2_temperaturevariability2023/physiology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{65AB8243-3E24-3340-9BB5-066A6F285CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0924A64-653D-4340-BFCF-A5BCE9D46517}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{65AB8243-3E24-3340-9BB5-066A6F285CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0916FFF7-A0CA-224E-B080-EDEBE37BF032}"/>
   <bookViews>
     <workbookView xWindow="300" yWindow="500" windowWidth="27640" windowHeight="15640" activeTab="1" xr2:uid="{D1FE7332-A6A1-B04B-AD65-B88218AD5A94}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="232">
   <si>
     <t>Metric</t>
   </si>
@@ -741,12 +741,51 @@
   <si>
     <t>Untreated:C:28-Treated:C:28</t>
   </si>
+  <si>
+    <t>Fv/Fm vs. Days at 32ºC</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Treatment</t>
+  </si>
+  <si>
+    <t>F-Statistic</t>
+  </si>
+  <si>
+    <t>Multiple R-Squared</t>
+  </si>
+  <si>
+    <t>Adjusted R-squared</t>
+  </si>
+  <si>
+    <t>Residual standard error</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>Acer</t>
+  </si>
+  <si>
+    <t>Untreated</t>
+  </si>
+  <si>
+    <t>Treated</t>
+  </si>
+  <si>
+    <t>Pcli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ED50 vs. Days at 32ºC </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -799,6 +838,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times Roman"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -820,7 +865,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -843,6 +888,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -858,6 +907,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4955,12 +5008,291 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2A14F9A-0824-5545-8C7A-D4B1D6AD7678}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="4" width="10.83203125" style="8"/>
+    <col min="5" max="6" width="17.1640625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" style="8" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1.1719999999999999</v>
+      </c>
+      <c r="D3" s="8">
+        <v>19</v>
+      </c>
+      <c r="E3" s="8">
+        <v>5.8110000000000002E-2</v>
+      </c>
+      <c r="F3" s="8">
+        <v>8.5380000000000005E-3</v>
+      </c>
+      <c r="G3" s="8">
+        <v>2.9839999999999998E-2</v>
+      </c>
+      <c r="H3" s="8">
+        <v>0.29249999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="C4" s="8">
+        <v>3.2590000000000001E-2</v>
+      </c>
+      <c r="D4" s="8">
+        <v>22</v>
+      </c>
+      <c r="E4" s="8">
+        <v>1.4790000000000001E-3</v>
+      </c>
+      <c r="F4" s="8">
+        <v>-4.3909999999999998E-2</v>
+      </c>
+      <c r="G4" s="8">
+        <v>4.6449999999999998E-2</v>
+      </c>
+      <c r="H4" s="8">
+        <v>0.85840000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="C5" s="8">
+        <v>9.1340000000000003</v>
+      </c>
+      <c r="D5" s="8">
+        <v>16</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0.3634</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0.3236</v>
+      </c>
+      <c r="G5" s="8">
+        <v>3.7310000000000003E-2</v>
+      </c>
+      <c r="H5" s="9">
+        <v>8.0949999999999998E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="C6" s="8">
+        <v>10.62</v>
+      </c>
+      <c r="D6" s="8">
+        <v>9</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0.54139999999999999</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0.4904</v>
+      </c>
+      <c r="G6" s="8">
+        <v>2.5729999999999999E-2</v>
+      </c>
+      <c r="H6" s="9">
+        <v>9.8449999999999996E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="8" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.3347</v>
+      </c>
+      <c r="D10" s="8">
+        <v>19</v>
+      </c>
+      <c r="E10" s="8">
+        <v>1.7309999999999999E-2</v>
+      </c>
+      <c r="F10" s="8">
+        <v>-3.4410000000000003E-2</v>
+      </c>
+      <c r="G10" s="8">
+        <v>0.13150000000000001</v>
+      </c>
+      <c r="H10" s="8">
+        <v>0.56969999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="C11" s="8">
+        <v>2.085E-2</v>
+      </c>
+      <c r="D11" s="8">
+        <v>22</v>
+      </c>
+      <c r="E11" s="10">
+        <v>9.4680000000000003E-4</v>
+      </c>
+      <c r="F11" s="8">
+        <v>-4.446E-2</v>
+      </c>
+      <c r="G11" s="8">
+        <v>0.183</v>
+      </c>
+      <c r="H11" s="8">
+        <v>0.88649999999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="C12" s="8">
+        <v>6.375</v>
+      </c>
+      <c r="D12" s="8">
+        <v>16</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0.28489999999999999</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0.2402</v>
+      </c>
+      <c r="G12" s="8">
+        <v>0.14419999999999999</v>
+      </c>
+      <c r="H12" s="9">
+        <v>2.2519999999999998E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="C13" s="8">
+        <v>46.44</v>
+      </c>
+      <c r="D13" s="8">
+        <v>9</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0.8377</v>
+      </c>
+      <c r="F13" s="8">
+        <v>0.8196</v>
+      </c>
+      <c r="G13" s="8">
+        <v>8.0699999999999994E-2</v>
+      </c>
+      <c r="H13" s="11">
+        <v>7.7750000000000006E-5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>